<commit_message>
Update Search Page Test Case
</commit_message>
<xml_diff>
--- a/src/main/java/cv_resources/Test_Data.xlsx
+++ b/src/main/java/cv_resources/Test_Data.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMS_Project\com.contentverse.dms\src\main\java\cv_resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462A599C-D310-49E6-AD36-FCE1B28C1179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F299172B-9174-4387-B550-F011AE8A69A7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="66">
   <si>
     <t>Username</t>
   </si>
@@ -53,9 +47,6 @@
     <t>browser</t>
   </si>
   <si>
-    <t>chrome</t>
-  </si>
-  <si>
     <t>url</t>
   </si>
   <si>
@@ -210,13 +201,40 @@
   </si>
   <si>
     <t>Implicit Wait</t>
+  </si>
+  <si>
+    <t>Custom Search</t>
+  </si>
+  <si>
+    <t>CustomDocumentType</t>
+  </si>
+  <si>
+    <t>DekstopReq-Form</t>
+  </si>
+  <si>
+    <t>CustomDocumentCreator</t>
+  </si>
+  <si>
+    <t>ajay</t>
+  </si>
+  <si>
+    <t>CustomDocName1</t>
+  </si>
+  <si>
+    <t>CustomDocName2</t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +255,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -259,12 +283,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -325,7 +351,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Display"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -377,7 +403,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Narrow"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -591,109 +617,109 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABFA8F24-ABFB-4BDB-B659-8A5BC2358C04}">
-  <dimension ref="A1:S13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.69921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.09765625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="26" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="30.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.59765625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="30.59765625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.09765625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.296875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.09765625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19">
       <c r="A1" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" t="s">
-        <v>9</v>
-      </c>
       <c r="I2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J2">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19">
       <c r="A3" s="2"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19">
       <c r="A4" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" t="s">
         <v>13</v>
       </c>
-      <c r="H4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" s="2"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19">
       <c r="A6" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>0</v>
@@ -702,160 +728,189 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F6" t="s">
         <v>2</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" t="s">
         <v>33</v>
       </c>
-      <c r="J6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19">
       <c r="A8" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" t="s">
         <v>17</v>
       </c>
-      <c r="F8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19">
       <c r="A10" s="2"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19">
       <c r="A11" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
         <v>19</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" t="s">
         <v>21</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="H11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="J11">
         <v>1000</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L11">
         <v>20</v>
       </c>
       <c r="M11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N11" t="s">
         <v>26</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O11" s="1" t="s">
+      <c r="P11" t="s">
         <v>28</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="R11" t="s">
         <v>30</v>
       </c>
-      <c r="R11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19">
       <c r="A13" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
         <v>35</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" t="s">
         <v>37</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="H13" t="s">
         <v>3</v>
       </c>
       <c r="I13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" t="s">
+        <v>53</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J13" t="s">
-        <v>54</v>
-      </c>
-      <c r="K13" s="1" t="s">
+      <c r="L13" t="s">
+        <v>52</v>
+      </c>
+      <c r="M13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="L13" t="s">
-        <v>53</v>
-      </c>
-      <c r="M13" s="1" t="s">
+      <c r="N13" t="s">
         <v>42</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="O13" s="1" t="s">
+      <c r="P13" t="s">
         <v>44</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="Q13" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="R13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S13" s="1"/>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>65</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revert "Update Search Page Test Case"
</commit_message>
<xml_diff>
--- a/src/main/java/cv_resources/Test_Data.xlsx
+++ b/src/main/java/cv_resources/Test_Data.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <workbookPr defaultThemeVersion="202300"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMS_Project\com.contentverse.dms\src\main\java\cv_resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462A599C-D310-49E6-AD36-FCE1B28C1179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F299172B-9174-4387-B550-F011AE8A69A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -30,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t>Username</t>
   </si>
@@ -47,6 +53,9 @@
     <t>browser</t>
   </si>
   <si>
+    <t>chrome</t>
+  </si>
+  <si>
     <t>url</t>
   </si>
   <si>
@@ -201,40 +210,13 @@
   </si>
   <si>
     <t>Implicit Wait</t>
-  </si>
-  <si>
-    <t>Custom Search</t>
-  </si>
-  <si>
-    <t>CustomDocumentType</t>
-  </si>
-  <si>
-    <t>DekstopReq-Form</t>
-  </si>
-  <si>
-    <t>CustomDocumentCreator</t>
-  </si>
-  <si>
-    <t>ajay</t>
-  </si>
-  <si>
-    <t>CustomDocName1</t>
-  </si>
-  <si>
-    <t>CustomDocName2</t>
-  </si>
-  <si>
-    <t>firefox</t>
-  </si>
-  <si>
-    <t>test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,12 +237,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -283,14 +259,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,7 +325,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -403,7 +377,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -617,109 +591,109 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABFA8F24-ABFB-4BDB-B659-8A5BC2358C04}">
+  <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.69921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.09765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.59765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="26" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.59765625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="30.59765625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.09765625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.296875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.09765625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J2">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
         <v>11</v>
       </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>0</v>
@@ -728,189 +702,160 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
         <v>2</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" t="s">
         <v>22</v>
       </c>
-      <c r="H11" t="s">
-        <v>21</v>
-      </c>
       <c r="I11" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J11">
         <v>1000</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L11">
         <v>20</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="R11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H13" t="s">
         <v>3</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J13" t="s">
+        <v>54</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L13" t="s">
         <v>53</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L13" t="s">
-        <v>52</v>
-      </c>
       <c r="M13" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="P13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Q13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R13" t="s">
         <v>45</v>
       </c>
-      <c r="R13" t="s">
-        <v>44</v>
-      </c>
       <c r="S13" s="1"/>
-    </row>
-    <row r="15" spans="1:19">
-      <c r="A15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>65</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changes Into Excel, WF (NOrmal,Dynamic) and add Email code also
</commit_message>
<xml_diff>
--- a/src/main/java/cv_resources/Test_Data.xlsx
+++ b/src/main/java/cv_resources/Test_Data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMS_Project\com.contentverse.dms\src\main\java\cv_resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462A599C-D310-49E6-AD36-FCE1B28C1179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C021CE22-413A-437C-AFB5-994475B3B0AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F299172B-9174-4387-B550-F011AE8A69A7}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F299172B-9174-4387-B550-F011AE8A69A7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CV_LoginTestCase" sheetId="1" r:id="rId1"/>
+    <sheet name="CV_DynamicTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="116">
   <si>
     <t>Username</t>
   </si>
@@ -143,42 +144,21 @@
     <t>Abc123def</t>
   </si>
   <si>
-    <t>WorkflowVerify_F_User</t>
-  </si>
-  <si>
     <t>shraddha</t>
   </si>
   <si>
-    <t>WorkflowVerify_F_Password</t>
-  </si>
-  <si>
     <t>root@123</t>
   </si>
   <si>
-    <t>WorkflowVerify_S_User</t>
-  </si>
-  <si>
-    <t>WorkflowVerify_S_Password</t>
-  </si>
-  <si>
     <t>DocumentName</t>
   </si>
   <si>
     <t>Name_OF_WF</t>
   </si>
   <si>
-    <t>ShradhaWorkflow</t>
-  </si>
-  <si>
-    <t>WorkflowStatus_By_First_User</t>
-  </si>
-  <si>
     <t>Accept</t>
   </si>
   <si>
-    <t>WorkflowStatus_By_Second_User</t>
-  </si>
-  <si>
     <t>Common</t>
   </si>
   <si>
@@ -210,13 +190,208 @@
   </si>
   <si>
     <t>Implicit Wait</t>
+  </si>
+  <si>
+    <t>Recent</t>
+  </si>
+  <si>
+    <t>Cabinet_Name</t>
+  </si>
+  <si>
+    <t>Drawer_Name</t>
+  </si>
+  <si>
+    <t>Folder_Name</t>
+  </si>
+  <si>
+    <t>Demo Ltd</t>
+  </si>
+  <si>
+    <t>Nikita</t>
+  </si>
+  <si>
+    <t>Test_load</t>
+  </si>
+  <si>
+    <t>WF_Verify_F_User</t>
+  </si>
+  <si>
+    <t>WF_Verify_F_Password</t>
+  </si>
+  <si>
+    <t>WF_Verify_S_User</t>
+  </si>
+  <si>
+    <t>WF_Verify_S_Password</t>
+  </si>
+  <si>
+    <t>ShradhaWF_</t>
+  </si>
+  <si>
+    <t>WF_Status_By_First_User</t>
+  </si>
+  <si>
+    <t>WF_Status_By_Second_User</t>
+  </si>
+  <si>
+    <t>Demo</t>
+  </si>
+  <si>
+    <t>User no</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>NameOfWF</t>
+  </si>
+  <si>
+    <t>NameOFDocument</t>
+  </si>
+  <si>
+    <t>Dynamic_WF_01</t>
+  </si>
+  <si>
+    <t>Document_Name</t>
+  </si>
+  <si>
+    <t>WorkFL_Name</t>
+  </si>
+  <si>
+    <t>First_Index</t>
+  </si>
+  <si>
+    <t>rajendra.mane</t>
+  </si>
+  <si>
+    <t>amol.thorat</t>
+  </si>
+  <si>
+    <t>New Index 4.1</t>
+  </si>
+  <si>
+    <t>New Index 5.1</t>
+  </si>
+  <si>
+    <t>New Index 6.1</t>
+  </si>
+  <si>
+    <t>http://192.168.3.17:8080/CVWeb/cvLgn</t>
+  </si>
+  <si>
+    <t>New Index 2.1</t>
+  </si>
+  <si>
+    <t>New Index 3.1</t>
+  </si>
+  <si>
+    <t>New Index 1.1 *</t>
+  </si>
+  <si>
+    <t>New Cabinet</t>
+  </si>
+  <si>
+    <t>Rajendra</t>
+  </si>
+  <si>
+    <t>DynamicWF</t>
+  </si>
+  <si>
+    <t>vinayakkumbhar</t>
+  </si>
+  <si>
+    <t>ketan.bhagat</t>
+  </si>
+  <si>
+    <t>mateen.shah</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>nikita.sawalkar</t>
+  </si>
+  <si>
+    <t>pankaj.wairagade</t>
+  </si>
+  <si>
+    <t>mayur.salunkhe</t>
+  </si>
+  <si>
+    <t>shradha.patil</t>
+  </si>
+  <si>
+    <t>suresh.agawane</t>
+  </si>
+  <si>
+    <t>name 1</t>
+  </si>
+  <si>
+    <t>name 2</t>
+  </si>
+  <si>
+    <t>name 3</t>
+  </si>
+  <si>
+    <t>name 4</t>
+  </si>
+  <si>
+    <t>name 5</t>
+  </si>
+  <si>
+    <t>name 6</t>
+  </si>
+  <si>
+    <t>name 7</t>
+  </si>
+  <si>
+    <t>name 8</t>
+  </si>
+  <si>
+    <t>name 9</t>
+  </si>
+  <si>
+    <t>name 10</t>
+  </si>
+  <si>
+    <t>name 11</t>
+  </si>
+  <si>
+    <t>name 12</t>
+  </si>
+  <si>
+    <t>name 13</t>
+  </si>
+  <si>
+    <t>name 14</t>
+  </si>
+  <si>
+    <t>name 15</t>
+  </si>
+  <si>
+    <t>Subjectt *</t>
+  </si>
+  <si>
+    <t>Office Note</t>
+  </si>
+  <si>
+    <t>kartik.korde</t>
+  </si>
+  <si>
+    <t>DynamicRJ_WF_24_05_01</t>
+  </si>
+  <si>
+    <t>Current User is last</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,6 +409,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -256,17 +439,41 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -599,41 +806,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABFA8F24-ABFB-4BDB-B659-8A5BC2358C04}">
-  <dimension ref="A1:S13"/>
+  <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="26" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="30.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
@@ -644,6 +853,974 @@
       <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="F2" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:19" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+    </row>
+    <row r="10" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="6">
+        <v>1000</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L11" s="6">
+        <v>20</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="O11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="R11" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+    </row>
+    <row r="13" spans="1:19" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q13" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="R13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="S13" s="8"/>
+    </row>
+    <row r="14" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>0</v>
+      </c>
+      <c r="B16" s="9">
+        <v>1</v>
+      </c>
+      <c r="C16" s="9">
+        <v>2</v>
+      </c>
+      <c r="D16" s="9">
+        <v>3</v>
+      </c>
+      <c r="E16" s="9">
+        <v>4</v>
+      </c>
+      <c r="F16" s="9">
+        <v>5</v>
+      </c>
+      <c r="G16" s="9">
+        <v>6</v>
+      </c>
+      <c r="H16" s="9">
+        <v>7</v>
+      </c>
+      <c r="I16" s="9">
+        <v>8</v>
+      </c>
+      <c r="J16" s="9">
+        <v>9</v>
+      </c>
+      <c r="K16" s="9">
+        <v>10</v>
+      </c>
+      <c r="L16" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" t="s">
+        <v>112</v>
+      </c>
+      <c r="G17" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" t="s">
+        <v>84</v>
+      </c>
+      <c r="I17" t="s">
+        <v>53</v>
+      </c>
+      <c r="J17" t="s">
+        <v>85</v>
+      </c>
+      <c r="K17" t="s">
+        <v>54</v>
+      </c>
+      <c r="L17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C24" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C27" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C28" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C29" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C30" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C31" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C32" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C33" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C34" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C35" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C36" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C37" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C38" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C39" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C40" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C41" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C42" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{60DC6B0A-4B98-4BB9-A657-CF0D618DC8AB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69991F65-9C60-4987-BBC2-C22EDA6689C7}">
+  <dimension ref="A1:R9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="18" width="13.42578125" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1"/>
+      <c r="C1"/>
+      <c r="D1"/>
+      <c r="E1"/>
+      <c r="F1"/>
+      <c r="G1"/>
+      <c r="H1"/>
+      <c r="I1"/>
+      <c r="J1"/>
+      <c r="K1"/>
+      <c r="L1"/>
+      <c r="M1"/>
+      <c r="N1"/>
+      <c r="O1"/>
+      <c r="P1"/>
+      <c r="Q1"/>
+      <c r="R1"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2"/>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F2" t="s">
         <v>7</v>
       </c>
@@ -654,20 +1831,45 @@
         <v>9</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="J2">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
+      <c r="B3"/>
       <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>48</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="B4"/>
       <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
@@ -686,15 +1888,42 @@
       <c r="H4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
+      <c r="B5"/>
       <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>49</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B6"/>
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
@@ -711,7 +1940,7 @@
         <v>32</v>
       </c>
       <c r="H6" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>33</v>
@@ -719,143 +1948,25 @@
       <c r="J6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J11">
-        <v>1000</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L11">
-        <v>20</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N11" t="s">
-        <v>27</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P11" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="R11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J13" t="s">
-        <v>54</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L13" t="s">
-        <v>53</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N13" t="s">
-        <v>43</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P13" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="R13" t="s">
-        <v>45</v>
-      </c>
-      <c r="S13" s="1"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+      <c r="O6"/>
+      <c r="P6"/>
+      <c r="Q6"/>
+      <c r="R6"/>
+    </row>
+    <row r="9" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="C9" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>71</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>